<commit_message>
Revert BEPEfCT to default settings
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
+++ b/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\ctrl-settings\BEPEfCT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="22035" windowHeight="11835"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BEPEfCT" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -104,6 +109,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -151,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,7 +194,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,49 +407,49 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -459,21 +467,23 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>